<commit_message>
Update results folder, with more ushort experiments, remove 5ushort and replace with a tar.gz version.
</commit_message>
<xml_diff>
--- a/results/OpenAIGym/Results.xlsx
+++ b/results/OpenAIGym/Results.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rhvt/Dev/BiSUNAOpenCL/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCDCD0F-5FAE-604A-B4C9-7B46BA5C5F32}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F70040A-873B-DB46-AB41-C6AA2900274A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="2860" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{DE3548C4-FDD8-E942-B840-C87F182DD8E1}"/>
+    <workbookView xWindow="-38400" yWindow="2400" windowWidth="38400" windowHeight="21600" xr2:uid="{DE3548C4-FDD8-E942-B840-C87F182DD8E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
-    <sheet name="CPU-Mountain-Float" sheetId="3" r:id="rId3"/>
-    <sheet name="CPU-Mountain-Bin" sheetId="1" r:id="rId4"/>
-    <sheet name="FPGA-Mountain-Bin" sheetId="2" r:id="rId5"/>
+    <sheet name="CPU-Mountain-Float" sheetId="3" r:id="rId2"/>
+    <sheet name="CPU-Mountain-Bin" sheetId="1" r:id="rId3"/>
+    <sheet name="FPGA-Mountain-Bin" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="101">
   <si>
     <t>Max</t>
   </si>
@@ -332,60 +331,6 @@
   </si>
   <si>
     <t>FPGA vs CPU TDP</t>
-  </si>
-  <si>
-    <t>VCU1525</t>
-  </si>
-  <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intel HD </t>
-  </si>
-  <si>
-    <t>GPU</t>
-  </si>
-  <si>
-    <t>Single Task</t>
-  </si>
-  <si>
-    <t>NDRange</t>
-  </si>
-  <si>
-    <t>Intel i7</t>
-  </si>
-  <si>
-    <t>Thread (8)</t>
-  </si>
-  <si>
-    <t>135sec</t>
-  </si>
-  <si>
-    <t>~300MHz</t>
-  </si>
-  <si>
-    <t>600sec</t>
-  </si>
-  <si>
-    <t>85W</t>
-  </si>
-  <si>
-    <t>75W</t>
-  </si>
-  <si>
-    <t>35sec</t>
-  </si>
-  <si>
-    <t>~1050MHz</t>
-  </si>
-  <si>
-    <t>2sec</t>
-  </si>
-  <si>
-    <t>~3GHz</t>
-  </si>
-  <si>
-    <t>Mountain Car (internal)</t>
   </si>
 </sst>
 </file>
@@ -783,7 +728,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -870,7 +815,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1290,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A499ADE4-6642-9146-BE97-0122C0A71E0E}">
   <dimension ref="B2:V35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1315,27 +1259,27 @@
       <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="43" t="s">
+      <c r="C3" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="43" t="s">
+      <c r="D3" s="43"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="43" t="s">
+      <c r="G3" s="44"/>
+      <c r="H3" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="45"/>
-      <c r="J3" s="43" t="s">
+      <c r="I3" s="44"/>
+      <c r="J3" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="45"/>
-      <c r="L3" s="43" t="s">
+      <c r="K3" s="44"/>
+      <c r="L3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="45"/>
+      <c r="M3" s="44"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B4" s="14" t="s">
@@ -1776,47 +1720,47 @@
         <v>61</v>
       </c>
       <c r="C13" s="36">
-        <f t="shared" ref="C13:M13" si="0">C28/(C22*1000)</f>
+        <f>C28/(C22*1000)</f>
         <v>2.04772</v>
       </c>
       <c r="D13" s="29">
-        <f t="shared" si="0"/>
+        <f>D28/(D22*1000)</f>
         <v>3.0557584615384612</v>
       </c>
       <c r="E13" s="26">
-        <f t="shared" si="0"/>
+        <f>E28/(E22*1000)</f>
         <v>88001.388562499997</v>
       </c>
       <c r="F13" s="30">
-        <f t="shared" si="0"/>
+        <f>F28/(F22*1000)</f>
         <v>3.4370353846153843</v>
       </c>
       <c r="G13" s="31">
-        <f t="shared" si="0"/>
+        <f>G28/(G22*1000)</f>
         <v>1712.766625</v>
       </c>
       <c r="H13" s="33">
-        <f t="shared" si="0"/>
+        <f>H28/(H22*1000)</f>
         <v>5.1965784615384614</v>
       </c>
       <c r="I13" s="31">
-        <f t="shared" si="0"/>
+        <f>I28/(I22*1000)</f>
         <v>1273.4642187500001</v>
       </c>
       <c r="J13" s="35">
-        <f t="shared" si="0"/>
+        <f>J28/(J22*1000)</f>
         <v>2.5790415384615386</v>
       </c>
       <c r="K13" s="26">
-        <f t="shared" si="0"/>
+        <f>K28/(K22*1000)</f>
         <v>1378.6822500000001</v>
       </c>
       <c r="L13" s="35">
-        <f t="shared" si="0"/>
+        <f>L28/(L22*1000)</f>
         <v>1.6049969230769232</v>
       </c>
       <c r="M13" s="26">
-        <f t="shared" si="0"/>
+        <f>M28/(M22*1000)</f>
         <v>785.49740625000004</v>
       </c>
     </row>
@@ -1825,47 +1769,47 @@
         <v>62</v>
       </c>
       <c r="C14" s="32">
-        <f t="shared" ref="C14:M14" si="1">C28/(C23*1000)</f>
+        <f>C28/(C23*1000)</f>
         <v>3.8029085714285711E-2</v>
       </c>
       <c r="D14" s="32">
-        <f t="shared" si="1"/>
+        <f>D28/(D23*1000)</f>
         <v>5.6749799999999996E-2</v>
       </c>
       <c r="E14" s="27">
-        <f t="shared" si="1"/>
+        <f>E28/(E23*1000)</f>
         <v>2395.6141505742235</v>
       </c>
       <c r="F14" s="28">
-        <f t="shared" si="1"/>
+        <f>F28/(F23*1000)</f>
         <v>6.3830657142857142E-2</v>
       </c>
       <c r="G14" s="27">
-        <f t="shared" si="1"/>
+        <f>G28/(G23*1000)</f>
         <v>46.6257184176946</v>
       </c>
       <c r="H14" s="28">
-        <f t="shared" si="1"/>
+        <f>H28/(H23*1000)</f>
         <v>9.6507885714285702E-2</v>
       </c>
       <c r="I14" s="27">
-        <f t="shared" si="1"/>
+        <f>I28/(I23*1000)</f>
         <v>34.666826882177794</v>
       </c>
       <c r="J14" s="28">
-        <f t="shared" si="1"/>
+        <f>J28/(J23*1000)</f>
         <v>4.7896485714285716E-2</v>
       </c>
       <c r="K14" s="27">
-        <f t="shared" si="1"/>
+        <f>K28/(K23*1000)</f>
         <v>37.531120374308806</v>
       </c>
       <c r="L14" s="28">
-        <f t="shared" si="1"/>
+        <f>L28/(L23*1000)</f>
         <v>2.9807085714285714E-2</v>
       </c>
       <c r="M14" s="27">
-        <f t="shared" si="1"/>
+        <f>M28/(M23*1000)</f>
         <v>21.383170565716718</v>
       </c>
     </row>
@@ -2378,47 +2322,47 @@
         <v>42</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:M33" si="2">C31/1000</f>
+        <f t="shared" ref="C33:M33" si="0">C31/1000</f>
         <v>10.300700000000001</v>
       </c>
       <c r="D33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>15.7302</v>
       </c>
       <c r="E33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>51.224199999999996</v>
       </c>
       <c r="F33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>12.8421</v>
       </c>
       <c r="G33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>123.9101</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>11.273299999999999</v>
       </c>
       <c r="I33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>147.61250000000001</v>
       </c>
       <c r="J33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>7.4592999999999998</v>
       </c>
       <c r="K33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>51.197800000000001</v>
       </c>
       <c r="L33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>3.9229000000000003</v>
       </c>
       <c r="M33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>41.960099999999997</v>
       </c>
     </row>
@@ -2442,194 +2386,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D171AC73-B227-DC42-A1C9-65A6B14ADA9B}">
-  <dimension ref="B1:H10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="42" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>106</v>
-      </c>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="42">
-        <v>100</v>
-      </c>
-      <c r="D6" s="42">
-        <v>100</v>
-      </c>
-      <c r="E6" s="42">
-        <v>100</v>
-      </c>
-      <c r="F6" s="42">
-        <v>100</v>
-      </c>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="42">
-        <v>-1000</v>
-      </c>
-      <c r="D7" s="42">
-        <v>-541</v>
-      </c>
-      <c r="E7" s="42">
-        <v>-1001</v>
-      </c>
-      <c r="F7" s="42">
-        <v>-351</v>
-      </c>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42">
-        <v>-203</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>109</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>114</v>
-      </c>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>113</v>
-      </c>
-      <c r="F9" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="42" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="D10" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" s="42" t="s">
-        <v>115</v>
-      </c>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42" t="s">
-        <v>117</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2F3F23-73AA-5A44-8B1A-63CD119A59DA}">
   <dimension ref="A2:AG215"/>
   <sheetViews>
@@ -13197,7 +12953,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E60D2105-5C86-474C-AEF4-0BBD7F940641}">
   <dimension ref="A3:AG2053"/>
   <sheetViews>
@@ -24095,7 +23851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D07D09-EF17-624B-A76C-8940DD9F981D}">
   <dimension ref="A2:AG215"/>
   <sheetViews>

</xml_diff>